<commit_message>
Major updates following addition of tests
</commit_message>
<xml_diff>
--- a/data/SimplifiedManifest_v1.0.xlsx
+++ b/data/SimplifiedManifest_v1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kr2/Documents/CGP/CGPaaS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kr2/GitLab/cgp_seq_input_val/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="12360" yWindow="460" windowWidth="24280" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="For entry" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <author>Keiran Raine</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,97 +54,6 @@
           </rPr>
           <t xml:space="preserve">
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>User info:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Please enter an identifier for your dataset</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>User info:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Use drop-down to select a valid response.
-Extra detail can be found on the ListData worksheet.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>User info:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Please select from drop-down list.
-Extra detail can be found on the ListData worksheet.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">User info:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Please select from drop-down list.
-Extra detail can be found on the ListData worksheet.</t>
         </r>
       </text>
     </comment>
@@ -157,16 +66,39 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">User info:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Only required for TGS (defaults to Y for others).  Please select from drop-down list.</t>
+          <t>User info:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Please enter an identifier for your dataset</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>User info:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Use drop-down to select a valid response.
+Extra detail can be found on the ListData worksheet.</t>
         </r>
       </text>
     </comment>
@@ -179,6 +111,74 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t>User info:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Please select from drop-down list.
+Extra detail can be found on the ListData worksheet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">User info:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Please select from drop-down list.
+Extra detail can be found on the ListData worksheet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">User info:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Only required for TGS (defaults to Y for others).  Please select from drop-down list.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">User Info:
 </t>
         </r>
@@ -192,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -224,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0">
+    <comment ref="D14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0">
+    <comment ref="E14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0">
+    <comment ref="F14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0">
+    <comment ref="G14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -411,7 +411,7 @@
     <author>Keiran Raine</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -434,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -456,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -478,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0">
+    <comment ref="A13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -601,7 +601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -632,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0">
+    <comment ref="D13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -664,7 +664,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -723,7 +723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="F13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -748,7 +748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0">
+    <comment ref="G13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -775,7 +775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>Your Ref:</t>
   </si>
@@ -982,6 +982,12 @@
       </rPr>
       <t xml:space="preserve"> can be submitted in a manifest.</t>
     </r>
+  </si>
+  <si>
+    <t>Mouse GRCm38, No chr prefix</t>
+  </si>
+  <si>
+    <t>Human GRCh37 + decoy v5 + NC_007605 (HPV), No chr prefix</t>
   </si>
 </sst>
 </file>
@@ -1238,43 +1244,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1289,6 +1273,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1570,11 +1576,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1588,1021 +1592,1024 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C7" s="28"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="25"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="25"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
+      <c r="A57" s="18"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="25"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="25"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="25"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="25"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="25"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
+      <c r="A65" s="18"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="25"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="25"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
+      <c r="A67" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="25"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="25"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
+      <c r="A70" s="18"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="25"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
+      <c r="A71" s="18"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="25"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="25"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
+      <c r="A73" s="18"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="25"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="25"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="25"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="25"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="25"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
+      <c r="A81" s="18"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="25"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="25"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="25"/>
+      <c r="A83" s="18"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="25"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="25"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="25"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="25"/>
+      <c r="A85" s="18"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="25"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="25"/>
+      <c r="A87" s="18"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="25"/>
+      <c r="A88" s="18"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="25"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="25"/>
+      <c r="A89" s="18"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="25"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
+      <c r="A90" s="18"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
+      <c r="A91" s="18"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="25"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
+      <c r="A92" s="18"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="25"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="25"/>
+      <c r="A93" s="18"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="25"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
+      <c r="A94" s="18"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="25"/>
-      <c r="B95" s="25"/>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="25"/>
+      <c r="A95" s="18"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="25"/>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="25"/>
+      <c r="A96" s="18"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="25"/>
-      <c r="B97" s="25"/>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="25"/>
+      <c r="A97" s="18"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="25"/>
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="25"/>
+      <c r="A98" s="18"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="25"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
-      <c r="G99" s="25"/>
+      <c r="A99" s="18"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="25"/>
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="25"/>
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="25"/>
+      <c r="A101" s="18"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="25"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="25"/>
-      <c r="B103" s="25"/>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="25"/>
+      <c r="A103" s="18"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="25"/>
-      <c r="B104" s="25"/>
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25"/>
+      <c r="A104" s="18"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="25"/>
-      <c r="B105" s="25"/>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="25"/>
+      <c r="A105" s="18"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="25"/>
-      <c r="B106" s="25"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="25"/>
+      <c r="A106" s="18"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="25"/>
-      <c r="B107" s="25"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="25"/>
+      <c r="A107" s="18"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="25"/>
-      <c r="B108" s="25"/>
-      <c r="C108" s="25"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="25"/>
-      <c r="F108" s="25"/>
-      <c r="G108" s="25"/>
+      <c r="A108" s="18"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="25"/>
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25"/>
+      <c r="A109" s="18"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="25"/>
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="25"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="25"/>
-      <c r="G110" s="25"/>
+      <c r="A110" s="18"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="18"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="18"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="18"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="18"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
     </row>
   </sheetData>
   <sheetProtection password="D3A7" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="7">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D110">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Y/N" sqref="C15:D114">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B8:C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B12:C12">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Y/N" sqref="C11:C110">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Y/N" sqref="E11:E110"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E15:E114"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2613,19 +2620,19 @@
           <x14:formula1>
             <xm:f>ListData!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:C5</xm:sqref>
+          <xm:sqref>B9:C9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail.">
           <x14:formula1>
             <xm:f>ListData!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:C6</xm:sqref>
+          <xm:sqref>B10:C10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail.">
           <x14:formula1>
             <xm:f>ListData!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:C7</xm:sqref>
+          <xm:sqref>B11:C11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2635,10 +2642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2653,317 +2660,323 @@
     <col min="8" max="8" width="116" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="C6" s="28"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
         <v>1</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="32">
+      <c r="F16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="12">
         <v>1</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="24" t="s">
+      <c r="B17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="D17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>2</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="F19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="14">
+        <v>2</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="14">
-        <v>1</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="14">
-        <v>2</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <v>1</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
-        <v>1</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="18">
-        <v>2</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="18">
-        <v>2</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="18" t="s">
+      <c r="F20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="20"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="27"/>
     </row>
   </sheetData>
   <sheetProtection password="D3A7" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="8">
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response" sqref="B5:C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response" sqref="B10:C10">
       <formula1>"DNA,RNA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B6:C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B11:C11">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from defined list:_x000d_WGS = Whole genome sequencing_x000d_WXS = Whole exome sequencing_x000d_TGS = Targeted Sequencing" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from defined list:_x000d_WGS = Whole genome sequencing_x000d_WXS = Whole exome sequencing_x000d_TGS = Targeted Sequencing" sqref="B9:C9">
       <formula1>"WGS,WXS,TGS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response." sqref="B3:C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response." sqref="B8:C8">
       <formula1>"HUMAN,MOUSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2976,11 +2989,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3009,7 +3025,9 @@
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
@@ -3027,7 +3045,9 @@
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Changes to mase manifest file
</commit_message>
<xml_diff>
--- a/data/SimplifiedManifest_v1.0.xlsx
+++ b/data/SimplifiedManifest_v1.0.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kr2/GitLab/cgp_seq_input_val/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kr2/volumes/kr2_vbox/GitHub/cgp_seq_input_val/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AD4AEC-263C-3C4C-BF53-A80F45F7A3D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="460" windowWidth="24280" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="12360" yWindow="460" windowWidth="24280" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For entry" sheetId="1" r:id="rId1"/>
     <sheet name="Example" sheetId="2" r:id="rId2"/>
     <sheet name="ListData" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Keiran Raine</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -111,21 +112,21 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>User info:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Please select from drop-down list.
+          <t xml:space="preserve">User info:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Please select from drop-down list.
 Extra detail can be found on the ListData worksheet.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -143,12 +144,33 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Please select from drop-down list.
-Extra detail can be found on the ListData worksheet.</t>
+          <t>Only required for TGS (defaults to Y for others).  Please select from drop-down list.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">User Info:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Groups samples together for analysis purposes.  e.g.  samples from the same Donor/Patient should share the same group value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -166,11 +188,21 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Only required for TGS (defaults to Y for others).  Please select from drop-down list.</t>
+          <t>Your sample identifier.  The mapping between this and the anonomised name will be provided.</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+This will not be held within Sanger databases and will only be available for a limited time in via manifest.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -179,20 +211,29 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">User Info:
+          <t>User info:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Groups samples together for analysis purposes.  e.g.  samples from the same Donor/Patient should share the same group value.</t>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Is this sample from normal tissue? Y/N</t>
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -210,21 +251,29 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Your sample identifier.  The mapping between this and the anonomised name will be provided.</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-This will not be held within Sanger databases and will only be available for a limited time in via manifest.</t>
+          <t xml:space="preserve">This sample will be considered the control' for any paired analysis.  </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <u/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Only 1 sample in a group can be selected for this state</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -233,128 +282,57 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>User info:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">User info:
 </t>
         </r>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Is this sample from normal tissue? Y/N</t>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>If multiple sequencing libraires were used tag each file with a common numerical id (only applies within a single sample).
+When unknown enter '</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>' (period).
+If multi-lane BAM/CRAM this information should be in the headers, enter '</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">' (period).
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">User info:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">This sample will be considered the control' for any paired analysis.  </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <u/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Only 1 sample in a group can be selected for this state</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">User info:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>If multiple sequencing libraires were used tag each file with a common numerical id (only applies within a single sample).
-When unknown enter '</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>' (period).
-If multi-lane BAM/CRAM this information should be in the headers, enter '</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">' (period).
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -379,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -406,12 +384,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Keiran Raine</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -434,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -456,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -478,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -503,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -525,7 +503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -547,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -569,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -601,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -632,7 +610,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -664,7 +642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -723,7 +701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -748,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -775,7 +753,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Your Ref:</t>
   </si>
@@ -908,31 +886,10 @@
     <t>Detail</t>
   </si>
   <si>
-    <t>Seq Protocol</t>
-  </si>
-  <si>
     <t>Species - Build</t>
   </si>
   <si>
-    <t>WXS</t>
-  </si>
-  <si>
-    <t>TGS</t>
-  </si>
-  <si>
-    <t>Whole genome sequenceing</t>
-  </si>
-  <si>
-    <t>Whole exome sequencing</t>
-  </si>
-  <si>
-    <t>Targeted sequencing</t>
-  </si>
-  <si>
     <t>Data Type</t>
-  </si>
-  <si>
-    <t>RNA</t>
   </si>
   <si>
     <r>
@@ -989,11 +946,47 @@
   <si>
     <t>Human GRCh37 + decoy v5 + NC_007605 (HPV), No chr prefix</t>
   </si>
+  <si>
+    <t>DNA:WGS</t>
+  </si>
+  <si>
+    <t>DNA:WXS</t>
+  </si>
+  <si>
+    <t>DNA:TGS</t>
+  </si>
+  <si>
+    <t>RNA:First strand</t>
+  </si>
+  <si>
+    <t>RNA:Second strand</t>
+  </si>
+  <si>
+    <t>RNA:Other</t>
+  </si>
+  <si>
+    <t>DNA Whole Genome Sequenceing</t>
+  </si>
+  <si>
+    <t>DNA Whole eXome Sequencing</t>
+  </si>
+  <si>
+    <t>DNA Targeted Sequencing</t>
+  </si>
+  <si>
+    <t>RNA first strand sequencing</t>
+  </si>
+  <si>
+    <t>RNA second strand sequencing</t>
+  </si>
+  <si>
+    <t>RNA other protocols</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1238,7 +1231,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1295,6 +1288,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1308,6 +1302,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1575,10 +1572,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1594,7 +1593,7 @@
     <row r="1" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14"/>
       <c r="B1" s="27" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -1646,59 +1645,61 @@
       <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
+      <c r="A10" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="26"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="26"/>
-    </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B13" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F13" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G13" s="22" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+    </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
@@ -2582,57 +2583,41 @@
       <c r="F113" s="18"/>
       <c r="G113" s="18"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="18"/>
-      <c r="B114" s="18"/>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-    </row>
   </sheetData>
-  <sheetProtection password="D3A7" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
-  <mergeCells count="7">
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
+  <mergeCells count="6">
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Y/N" sqref="C15:D114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Y/N" sqref="C14:D113" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B12:C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B11:C11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E15:E114"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E14:E113" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail.">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail." xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>ListData!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B9:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail." xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
-            <xm:f>ListData!$D$2:$D$4</xm:f>
+            <xm:f>ListData!$D$2:$D$7</xm:f>
           </x14:formula1>
           <xm:sqref>B10:C10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from drop-down list.  See ListData worksheet for more detail.">
-          <x14:formula1>
-            <xm:f>ListData!$G$2:$G$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B11:C11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2641,7 +2626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2967,16 +2952,16 @@
     <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response" sqref="B10:C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response" sqref="B10:C10" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"DNA,RNA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B11:C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Only required for TGS (entry ignored for others, defaulted to Y).  Please select from defined list" sqref="B11:C11" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from defined list:_x000d_WGS = Whole genome sequencing_x000d_WXS = Whole exome sequencing_x000d_TGS = Targeted Sequencing" sqref="B9:C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Please select from defined list:_x000d_WGS = Whole genome sequencing_x000d_WXS = Whole exome sequencing_x000d_TGS = Targeted Sequencing" sqref="B9:C9" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"WGS,WXS,TGS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response." sqref="B8:C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User info:" prompt="Use drop-down to select a valid response." sqref="B8:C8" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"HUMAN,MOUSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2986,91 +2971,96 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>49</v>
+      <c r="E7" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="D3A7" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reject file names with "#" in manifest validate
</commit_message>
<xml_diff>
--- a/data/SimplifiedManifest_v1.0.xlsx
+++ b/data/SimplifiedManifest_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kr2/volumes/kr2_vbox/GitHub/cgp_seq_input_val/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yx2/Documents/projects/cgp_seq_input_val/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BFC3A7-21C9-4447-A34D-0563625A3502}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A94065B-2C97-C446-B537-669D08B8D106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="460" windowWidth="24280" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3160" yWindow="440" windowWidth="24280" windowHeight="23460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For entry" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User Info:
 </t>
@@ -53,6 +54,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Completed by Automated System</t>
         </r>
@@ -61,6 +63,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -75,6 +78,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
@@ -83,6 +87,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -92,6 +97,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Please enter an identifier for your dataset</t>
         </r>
@@ -105,6 +111,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
@@ -113,6 +120,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -122,6 +130,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Use drop-down to select a valid response.
 </t>
@@ -131,6 +140,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Extra detail can be found on the ListData worksheet.</t>
         </r>
@@ -144,6 +154,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -153,6 +164,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Please select from drop-down list.
 </t>
@@ -162,6 +174,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Extra detail can be found on the ListData worksheet.</t>
         </r>
@@ -175,6 +188,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -184,6 +198,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Only required for TGS (defaults to Y for others).  Please select from drop-down list.</t>
         </r>
@@ -197,6 +212,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User Info:
 </t>
@@ -206,6 +222,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Groups samples together for analysis purposes.  e.g.  samples from the same Donor/Patient should share the same group value.</t>
         </r>
@@ -219,6 +236,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -228,6 +246,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Your sample identifier.  You are responsible for ensuring this is anonymised appropriately.</t>
         </r>
@@ -241,6 +260,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
@@ -249,6 +269,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -258,6 +279,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Is this sample from normal tissue? Y/N</t>
         </r>
@@ -271,6 +293,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -280,6 +303,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">This sample will be considered the control' for any paired analysis.  </t>
         </r>
@@ -290,6 +314,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Only 1 sample in a group can be selected for this state</t>
         </r>
@@ -298,6 +323,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>.</t>
         </r>
@@ -311,6 +337,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -320,6 +347,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">If multiple sequencing libraires were used tag each file with a common numerical id (only applies within a single sample).
 </t>
@@ -329,6 +357,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>When unknown enter '</t>
         </r>
@@ -338,6 +367,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>.</t>
         </r>
@@ -346,6 +376,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">' (period).
 </t>
@@ -355,6 +386,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>If multi-lane BAM/CRAM this information should be in the headers, enter '</t>
         </r>
@@ -364,6 +396,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>.</t>
         </r>
@@ -372,6 +405,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">' (period).
 </t>
@@ -386,6 +420,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -395,6 +430,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">bam, cram {fq,fastq}.{gz,bz2} interleaved file.
 </t>
@@ -404,6 +440,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">OR
 </t>
@@ -413,8 +450,19 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-          </rPr>
-          <t>{fq,fastq}.{gz,{bz2} read 1 file.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">{fq,fastq}.{gz,{bz2} read 1 file.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>'#' is not allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -426,6 +474,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
@@ -434,6 +483,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -443,8 +493,19 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-          </rPr>
-          <t>Only applicable for {fq,fastq}.{gz,bz2} read 2.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Only applicable for {fq,fastq}.{gz,bz2} read 2.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>'#' is not allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -466,6 +527,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User Info:
 Completed by Automated System</t>
@@ -475,6 +537,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -489,6 +552,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
@@ -497,6 +561,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Please enter an identifier for your dataset</t>
@@ -511,6 +576,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
@@ -519,6 +585,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Use drop-down to select a valid response</t>
@@ -533,6 +600,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -542,6 +610,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Use drop-down to select a valid response</t>
         </r>
@@ -555,6 +624,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -564,19 +634,21 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Only equired for TGS (defaults to Y for others).  Please select from defined list</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{B37CDFAE-C0D2-664F-8FF6-C51E354E6763}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User Info:
 </t>
@@ -584,21 +656,23 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Groups samples together for analysis purposes.  e.g.  samples from the same Donor/Patient should share the same group value.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{B19FC50C-6E6E-3544-838F-AA4E36F243DB}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -606,62 +680,56 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Your sample identifier.  The mapping between this and the anonomised name will be provided.</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-This will not be held within Sanger databases and will only be available for a limited time in via manifest.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Your sample identifier.  You are responsible for ensuring this is anonymised appropriately.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{89DB5CBE-5425-F346-AA81-43815E34A556}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Is this sample from normal tissue? Y/N</t>
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{A5E78F79-DD41-B447-8562-BC7ACB1AD903}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -669,8 +737,9 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">This sample will be considered the control' for any paired analysis.  </t>
         </r>
@@ -679,21 +748,32 @@
             <i/>
             <u/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Only 1 sample in a group can be selected for this state.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Only 1 sample in a group can be selected for this state</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{F0F1C73F-AD7A-F548-BF7B-1DAD612D8DE8}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -701,58 +781,82 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>If multiple sequencing libraires were used tag each file with a common numerical id (only applies within a single sample).
-When unknown enter '</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If multiple sequencing libraires were used tag each file with a common numerical id (only applies within a single sample).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>When unknown enter '</t>
         </r>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>.</t>
         </r>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>' (period).
-If multi-lane BAM/CRAM this information should be in the headers, enter '</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">' (period).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>If multi-lane BAM/CRAM this information should be in the headers, enter '</t>
         </r>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>.</t>
         </r>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">' (period).
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{7A7D683D-8937-E34E-86EE-52657670A35F}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">User info:
 </t>
@@ -760,35 +864,84 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">BAM, CRAM, FASTQ[.gz] interleaved file.
-OR
-FASTQ[.gz] read 1 file.
-</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">bam, cram {fq,fastq}.{gz,bz2} interleaved file.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OR
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">{fq,fastq}.{gz,{bz2} read 1 file.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>'#' is not allowed in the file name.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{6AB15F99-371A-1B48-AC51-A0D5C55C72AF}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>User info:</t>
         </r>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Only applicable for FASTQ[.gz] read 2.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Only applicable for {fq,fastq}.{gz,bz2} read 2.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>'#' is not allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -1025,7 +1178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1045,19 +1198,14 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1087,11 +1235,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1099,6 +1249,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1139,7 +1290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1158,17 +1309,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1279,26 +1419,25 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1308,12 +1447,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -1330,16 +1469,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1628,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="A13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1644,27 +1783,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14"/>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1672,972 +1811,972 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="26"/>
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
+      <c r="A67" s="17"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="18"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
+      <c r="A73" s="17"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
+      <c r="A74" s="17"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="18"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
+      <c r="A75" s="17"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
+      <c r="A76" s="17"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="18"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
+      <c r="A77" s="17"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="18"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
+      <c r="A78" s="17"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18"/>
+      <c r="A79" s="17"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="18"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="18"/>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
+      <c r="A81" s="17"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="17"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="18"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="18"/>
+      <c r="A83" s="17"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="18"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
+      <c r="A84" s="17"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
+      <c r="A85" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="18"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="18"/>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
+      <c r="A87" s="17"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
+      <c r="A88" s="17"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="18"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
+      <c r="A89" s="17"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="18"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
+      <c r="A90" s="17"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="18"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="18"/>
+      <c r="A91" s="17"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
+      <c r="G91" s="17"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="18"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
+      <c r="A92" s="17"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="18"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="18"/>
+      <c r="A93" s="17"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="17"/>
+      <c r="G93" s="17"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="18"/>
-      <c r="B94" s="18"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
+      <c r="A94" s="17"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="17"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="18"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
+      <c r="A95" s="17"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="18"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="18"/>
+      <c r="A96" s="17"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="18"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
+      <c r="A97" s="17"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="18"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
+      <c r="A98" s="17"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="18"/>
-      <c r="B99" s="18"/>
-      <c r="C99" s="18"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="18"/>
+      <c r="A99" s="17"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="17"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="18"/>
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
+      <c r="A100" s="17"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="18"/>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="18"/>
+      <c r="A101" s="17"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="18"/>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
+      <c r="A102" s="17"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="18"/>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
+      <c r="A103" s="17"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="17"/>
+      <c r="G103" s="17"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="18"/>
-      <c r="B104" s="18"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
+      <c r="A104" s="17"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="17"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="18"/>
-      <c r="B105" s="18"/>
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
+      <c r="A105" s="17"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="17"/>
+      <c r="G105" s="17"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="18"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
+      <c r="A106" s="17"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="18"/>
-      <c r="B107" s="18"/>
-      <c r="C107" s="18"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="18"/>
+      <c r="A107" s="17"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="17"/>
+      <c r="G107" s="17"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="18"/>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="18"/>
+      <c r="A108" s="17"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="17"/>
+      <c r="G108" s="17"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="18"/>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="18"/>
-      <c r="E109" s="18"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="18"/>
+      <c r="A109" s="17"/>
+      <c r="B109" s="17"/>
+      <c r="C109" s="17"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="17"/>
+      <c r="G109" s="17"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="18"/>
-      <c r="B110" s="18"/>
-      <c r="C110" s="18"/>
-      <c r="D110" s="18"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="18"/>
+      <c r="A110" s="17"/>
+      <c r="B110" s="17"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="17"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="18"/>
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="18"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="18"/>
+      <c r="A111" s="17"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="17"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="17"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="18"/>
-      <c r="B112" s="18"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="18"/>
-      <c r="F112" s="18"/>
-      <c r="G112" s="18"/>
+      <c r="A112" s="17"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="17"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="18"/>
-      <c r="B113" s="18"/>
-      <c r="C113" s="18"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="18"/>
+      <c r="A113" s="17"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="17"/>
+      <c r="D113" s="17"/>
+      <c r="E113" s="17"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="k12N+EGVTUbfY4Mj1FCr3XjQacH8Qp6e785xgoWQfipleOTejr75XJHeWZt5Q/Cys+72GgHg+Qp4zgp8l/lGBA==" saltValue="NOChLvd9f+Wz3IfCaz1FUQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3TQ1ycMP9gR3EkOcQ2GEB1CYqh2eUmjp4kE6JLBrbd1ALHlC4DAAQjqsbuJ7ur/x4UHRrfghibGv/MHTe/b9lA==" saltValue="YbC4JfnQNIeicECuwELXcg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="6">
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
@@ -2682,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2702,13 +2841,13 @@
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2716,16 +2855,16 @@
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="28"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -2734,10 +2873,10 @@
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2746,10 +2885,10 @@
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="26"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -2758,10 +2897,10 @@
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2772,10 +2911,10 @@
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -2793,193 +2932,193 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>1</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="30" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>1</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>1</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="31"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="30"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>1</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>2</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="31"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <v>1</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="31"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="13">
+      <c r="A17" s="12">
         <v>1</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="32"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <v>2</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="33" t="s">
+      <c r="G18" s="13"/>
+      <c r="H18" s="32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <v>2</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="28"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9oa5VqhKXfY56CuNArOvy1YE6kYJx7aPWZSOz15M3GNKH2aFZ2UBcx9blfAFY2e0bsj4ubOHtB0+ku6lqQ4E1Q==" saltValue="XRf0qHz9rm56iyBgg/EY9A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="P+fRLSjRmzG6PViq19so0RITc1dJkjgzu8IrnuPeXc5j5jiMaROY6dVZpxzeAY8Y6uv4R7f/qLuMLAW3OcCxQA==" saltValue="BVJM725WonDD3j7P0R5VLQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="7">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="H13:H17"/>
@@ -3079,26 +3218,26 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="25" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated excel files comments to let user know the allowed characters in filenames
</commit_message>
<xml_diff>
--- a/data/SimplifiedManifest_v1.0.xlsx
+++ b/data/SimplifiedManifest_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yx2/Documents/projects/cgp_seq_input_val/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A94065B-2C97-C446-B537-669D08B8D106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEA2609-F2C1-DC41-A829-8C17276EDA52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="440" windowWidth="24280" windowHeight="23460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3160" yWindow="440" windowWidth="24280" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For entry" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,26 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>'#' is not allowed in the file name.</t>
+          <t xml:space="preserve">Only characters in </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[a-zA-Z0-9._+-] are</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -502,10 +521,28 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>'#' is not allowed in the file name.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Only characters in </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[a-zA-Z0-9._+-] are</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -640,7 +677,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{B37CDFAE-C0D2-664F-8FF6-C51E354E6763}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{FB85D061-21FD-BC40-804A-C6BE4F4F5B72}">
       <text>
         <r>
           <rPr>
@@ -664,7 +701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{B19FC50C-6E6E-3544-838F-AA4E36F243DB}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{ECAC3824-D6A8-C44C-9374-EC737DF5E685}">
       <text>
         <r>
           <rPr>
@@ -688,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{89DB5CBE-5425-F346-AA81-43815E34A556}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{DC08E677-77D1-1F4F-AFDB-D12924F95679}">
       <text>
         <r>
           <rPr>
@@ -721,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{A5E78F79-DD41-B447-8562-BC7ACB1AD903}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{D3F0EE26-3567-1642-BAB8-B905A6E2B3F4}">
       <text>
         <r>
           <rPr>
@@ -765,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{F0F1C73F-AD7A-F548-BF7B-1DAD612D8DE8}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{EB062248-4E8B-8640-A873-81D2C6546A5D}">
       <text>
         <r>
           <rPr>
@@ -848,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{7A7D683D-8937-E34E-86EE-52657670A35F}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{97AE82D0-FABE-554E-95ED-FB6F88F23BD3}">
       <text>
         <r>
           <rPr>
@@ -898,11 +935,30 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>'#' is not allowed in the file name.</t>
+          <t xml:space="preserve">Only characters in </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[a-zA-Z0-9._+-] are</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> allowed in the file name.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{6AB15F99-371A-1B48-AC51-A0D5C55C72AF}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{E2385E4E-84B3-E541-B42C-EB3CCB0BC376}">
       <text>
         <r>
           <rPr>
@@ -938,10 +994,28 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>'#' is not allowed in the file name.</t>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Only characters in </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[a-zA-Z0-9._+-] are</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -1178,7 +1252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1250,6 +1324,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="+mn-lt"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1767,11 +1854,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="A13:G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -1782,7 +1869,7 @@
     <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="122" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="122" customHeight="1">
       <c r="A1" s="13"/>
       <c r="B1" s="27" t="s">
         <v>39</v>
@@ -1793,13 +1880,13 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1807,7 +1894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1815,35 +1902,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="28"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1852,7 +1939,7 @@
       </c>
       <c r="C11" s="26"/>
     </row>
-    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="17" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>6</v>
       </c>
@@ -1875,7 +1962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -1884,7 +1971,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -1893,7 +1980,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -1902,7 +1989,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1911,7 +1998,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1920,7 +2007,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1929,7 +2016,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -1938,7 +2025,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1947,7 +2034,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1956,7 +2043,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1965,7 +2052,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1974,7 +2061,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1983,7 +2070,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -1992,7 +2079,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -2001,7 +2088,7 @@
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -2010,7 +2097,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -2019,7 +2106,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -2028,7 +2115,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -2037,7 +2124,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2046,7 +2133,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -2055,7 +2142,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -2064,7 +2151,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -2073,7 +2160,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -2082,7 +2169,7 @@
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -2091,7 +2178,7 @@
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -2100,7 +2187,7 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -2109,7 +2196,7 @@
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -2118,7 +2205,7 @@
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -2127,7 +2214,7 @@
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
@@ -2136,7 +2223,7 @@
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -2145,7 +2232,7 @@
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
@@ -2154,7 +2241,7 @@
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
@@ -2163,7 +2250,7 @@
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -2172,7 +2259,7 @@
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -2181,7 +2268,7 @@
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -2190,7 +2277,7 @@
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -2199,7 +2286,7 @@
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -2208,7 +2295,7 @@
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2217,7 +2304,7 @@
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -2226,7 +2313,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -2235,7 +2322,7 @@
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -2244,7 +2331,7 @@
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -2253,7 +2340,7 @@
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -2262,7 +2349,7 @@
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -2271,7 +2358,7 @@
       <c r="F57" s="17"/>
       <c r="G57" s="17"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -2280,7 +2367,7 @@
       <c r="F58" s="17"/>
       <c r="G58" s="17"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -2289,7 +2376,7 @@
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -2298,7 +2385,7 @@
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -2307,7 +2394,7 @@
       <c r="F61" s="17"/>
       <c r="G61" s="17"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -2316,7 +2403,7 @@
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -2325,7 +2412,7 @@
       <c r="F63" s="17"/>
       <c r="G63" s="17"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -2334,7 +2421,7 @@
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="17"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -2343,7 +2430,7 @@
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -2352,7 +2439,7 @@
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" s="17"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -2361,7 +2448,7 @@
       <c r="F67" s="17"/>
       <c r="G67" s="17"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -2370,7 +2457,7 @@
       <c r="F68" s="17"/>
       <c r="G68" s="17"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -2379,7 +2466,7 @@
       <c r="F69" s="17"/>
       <c r="G69" s="17"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -2388,7 +2475,7 @@
       <c r="F70" s="17"/>
       <c r="G70" s="17"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -2397,7 +2484,7 @@
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -2406,7 +2493,7 @@
       <c r="F72" s="17"/>
       <c r="G72" s="17"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -2415,7 +2502,7 @@
       <c r="F73" s="17"/>
       <c r="G73" s="17"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -2424,7 +2511,7 @@
       <c r="F74" s="17"/>
       <c r="G74" s="17"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -2433,7 +2520,7 @@
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -2442,7 +2529,7 @@
       <c r="F76" s="17"/>
       <c r="G76" s="17"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" s="17"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -2451,7 +2538,7 @@
       <c r="F77" s="17"/>
       <c r="G77" s="17"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -2460,7 +2547,7 @@
       <c r="F78" s="17"/>
       <c r="G78" s="17"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" s="17"/>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -2469,7 +2556,7 @@
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -2478,7 +2565,7 @@
       <c r="F80" s="17"/>
       <c r="G80" s="17"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -2487,7 +2574,7 @@
       <c r="F81" s="17"/>
       <c r="G81" s="17"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" s="17"/>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -2496,7 +2583,7 @@
       <c r="F82" s="17"/>
       <c r="G82" s="17"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" s="17"/>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -2505,7 +2592,7 @@
       <c r="F83" s="17"/>
       <c r="G83" s="17"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -2514,7 +2601,7 @@
       <c r="F84" s="17"/>
       <c r="G84" s="17"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" s="17"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -2523,7 +2610,7 @@
       <c r="F85" s="17"/>
       <c r="G85" s="17"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" s="17"/>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -2532,7 +2619,7 @@
       <c r="F86" s="17"/>
       <c r="G86" s="17"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" s="17"/>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -2541,7 +2628,7 @@
       <c r="F87" s="17"/>
       <c r="G87" s="17"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" s="17"/>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -2550,7 +2637,7 @@
       <c r="F88" s="17"/>
       <c r="G88" s="17"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -2559,7 +2646,7 @@
       <c r="F89" s="17"/>
       <c r="G89" s="17"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" s="17"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -2568,7 +2655,7 @@
       <c r="F90" s="17"/>
       <c r="G90" s="17"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" s="17"/>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -2577,7 +2664,7 @@
       <c r="F91" s="17"/>
       <c r="G91" s="17"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -2586,7 +2673,7 @@
       <c r="F92" s="17"/>
       <c r="G92" s="17"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" s="17"/>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -2595,7 +2682,7 @@
       <c r="F93" s="17"/>
       <c r="G93" s="17"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" s="17"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -2604,7 +2691,7 @@
       <c r="F94" s="17"/>
       <c r="G94" s="17"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" s="17"/>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -2613,7 +2700,7 @@
       <c r="F95" s="17"/>
       <c r="G95" s="17"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" s="17"/>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -2622,7 +2709,7 @@
       <c r="F96" s="17"/>
       <c r="G96" s="17"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" s="17"/>
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
@@ -2631,7 +2718,7 @@
       <c r="F97" s="17"/>
       <c r="G97" s="17"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" s="17"/>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
@@ -2640,7 +2727,7 @@
       <c r="F98" s="17"/>
       <c r="G98" s="17"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" s="17"/>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -2649,7 +2736,7 @@
       <c r="F99" s="17"/>
       <c r="G99" s="17"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -2658,7 +2745,7 @@
       <c r="F100" s="17"/>
       <c r="G100" s="17"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" s="17"/>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -2667,7 +2754,7 @@
       <c r="F101" s="17"/>
       <c r="G101" s="17"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" s="17"/>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>
@@ -2676,7 +2763,7 @@
       <c r="F102" s="17"/>
       <c r="G102" s="17"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
       <c r="C103" s="17"/>
@@ -2685,7 +2772,7 @@
       <c r="F103" s="17"/>
       <c r="G103" s="17"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" s="17"/>
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
@@ -2694,7 +2781,7 @@
       <c r="F104" s="17"/>
       <c r="G104" s="17"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" s="17"/>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
@@ -2703,7 +2790,7 @@
       <c r="F105" s="17"/>
       <c r="G105" s="17"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" s="17"/>
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
@@ -2712,7 +2799,7 @@
       <c r="F106" s="17"/>
       <c r="G106" s="17"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" s="17"/>
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
@@ -2721,7 +2808,7 @@
       <c r="F107" s="17"/>
       <c r="G107" s="17"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" s="17"/>
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
@@ -2730,7 +2817,7 @@
       <c r="F108" s="17"/>
       <c r="G108" s="17"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" s="17"/>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -2739,7 +2826,7 @@
       <c r="F109" s="17"/>
       <c r="G109" s="17"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>
@@ -2748,7 +2835,7 @@
       <c r="F110" s="17"/>
       <c r="G110" s="17"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" s="17"/>
       <c r="B111" s="17"/>
       <c r="C111" s="17"/>
@@ -2757,7 +2844,7 @@
       <c r="F111" s="17"/>
       <c r="G111" s="17"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" s="17"/>
       <c r="B112" s="17"/>
       <c r="C112" s="17"/>
@@ -2766,7 +2853,7 @@
       <c r="F112" s="17"/>
       <c r="G112" s="17"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
@@ -2776,7 +2863,7 @@
       <c r="G113" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3TQ1ycMP9gR3EkOcQ2GEB1CYqh2eUmjp4kE6JLBrbd1ALHlC4DAAQjqsbuJ7ur/x4UHRrfghibGv/MHTe/b9lA==" saltValue="YbC4JfnQNIeicECuwELXcg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2BQWyI+GIPjSwsU51Ogr+zLsNy5hAFSwqNsPq1vw6A5/a/XFm/VZ4Xc41hWVW32h4ZkenK5X6rLMsaQfU8pNtQ==" saltValue="Sq/9h6z2nEPgl7nKKj84LA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="6">
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
@@ -2821,11 +2908,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -2837,13 +2924,13 @@
     <col min="8" max="8" width="116" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -2851,7 +2938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2859,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="28" t="s">
         <v>9</v>
@@ -2869,7 +2956,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +2968,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -2893,7 +2980,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -2907,7 +2994,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -2921,7 +3008,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2931,7 +3018,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="17" thickBot="1">
       <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
@@ -2957,7 +3044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="8">
         <v>1</v>
       </c>
@@ -2981,7 +3068,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="9">
         <v>1</v>
       </c>
@@ -3003,7 +3090,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="10">
         <v>1</v>
       </c>
@@ -3025,7 +3112,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="11">
         <v>1</v>
       </c>
@@ -3047,7 +3134,7 @@
       <c r="G16" s="11"/>
       <c r="H16" s="30"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="12">
         <v>1</v>
       </c>
@@ -3071,7 +3158,7 @@
       </c>
       <c r="H17" s="31"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="13">
         <v>2</v>
       </c>
@@ -3095,7 +3182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="13">
         <v>2</v>
       </c>
@@ -3118,7 +3205,7 @@
       <c r="H19" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="P+fRLSjRmzG6PViq19so0RITc1dJkjgzu8IrnuPeXc5j5jiMaROY6dVZpxzeAY8Y6uv4R7f/qLuMLAW3OcCxQA==" saltValue="BVJM725WonDD3j7P0R5VLQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="lVUwAhUpZTUAX50Ot5Prt8PYULKNg3NtpKdPBaOeagqhKnol17l4WIl/dJJv2G76kkSWu86USO9WG46WRjKGkQ==" saltValue="CessEHmGHbjq3udPHj78Bw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="7">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="H13:H17"/>
@@ -3159,7 +3246,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.5" bestFit="1" customWidth="1"/>
@@ -3167,7 +3254,7 @@
     <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -3181,7 +3268,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -3195,7 +3282,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3209,7 +3296,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="D4" s="1" t="s">
         <v>44</v>
       </c>
@@ -3217,7 +3304,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="D5" s="25" t="s">
         <v>45</v>
       </c>
@@ -3225,7 +3312,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="D6" s="25" t="s">
         <v>46</v>
       </c>
@@ -3233,7 +3320,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="D7" s="25" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
removed "+" from CWL allowed filename pattern, updated comments in excel manifests
</commit_message>
<xml_diff>
--- a/data/SimplifiedManifest_v1.0.xlsx
+++ b/data/SimplifiedManifest_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yx2/Documents/projects/cgp_seq_input_val/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEA2609-F2C1-DC41-A829-8C17276EDA52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15526F34-DDC8-F043-80BB-F83820FA6C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="440" windowWidth="24280" windowHeight="23460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3160" yWindow="440" windowWidth="24280" windowHeight="23460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For entry" sheetId="1" r:id="rId1"/>
@@ -462,26 +462,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Only characters in </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[a-zA-Z0-9._+-] are</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> allowed in the file name.</t>
+          <t>Only characters in [a-zA-Z0-9._-] are allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -524,25 +505,7 @@
             <rFont val="+mn-lt"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Only characters in </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t>[a-zA-Z0-9._+-] are</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> allowed in the file name.</t>
+          <t>Only characters in [a-zA-Z0-9._-] are allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -677,7 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{FB85D061-21FD-BC40-804A-C6BE4F4F5B72}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{0D2FE8CE-1D1D-E94E-B95A-7964E278F1D0}">
       <text>
         <r>
           <rPr>
@@ -701,7 +664,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{ECAC3824-D6A8-C44C-9374-EC737DF5E685}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{683EACB8-8F67-8E41-B5F2-8C617C402BCB}">
       <text>
         <r>
           <rPr>
@@ -725,7 +688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{DC08E677-77D1-1F4F-AFDB-D12924F95679}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{3BB1734B-08BB-7842-A6FD-E10A35D91E5A}">
       <text>
         <r>
           <rPr>
@@ -758,7 +721,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{D3F0EE26-3567-1642-BAB8-B905A6E2B3F4}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{58C987F0-27D6-514D-82D8-3C9A87FFB701}">
       <text>
         <r>
           <rPr>
@@ -802,7 +765,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{EB062248-4E8B-8640-A873-81D2C6546A5D}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{D459608E-957A-F840-B9E0-12EF91E9A6F8}">
       <text>
         <r>
           <rPr>
@@ -885,7 +848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{97AE82D0-FABE-554E-95ED-FB6F88F23BD3}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{68496FC9-A98C-F54E-9C18-2B2ED386793A}">
       <text>
         <r>
           <rPr>
@@ -935,30 +898,11 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Only characters in </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[a-zA-Z0-9._+-] are</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> allowed in the file name.</t>
+          <t>Only characters in [a-zA-Z0-9._-] are allowed in the file name.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{E2385E4E-84B3-E541-B42C-EB3CCB0BC376}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{006C43F5-84DD-BC47-BCCA-D3A0C8B56FD7}">
       <text>
         <r>
           <rPr>
@@ -997,25 +941,7 @@
             <rFont val="+mn-lt"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Only characters in </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t>[a-zA-Z0-9._+-] are</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="+mn-lt"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> allowed in the file name.</t>
+          <t>Only characters in [a-zA-Z0-9._-] are allowed in the file name.</t>
         </r>
       </text>
     </comment>
@@ -1252,7 +1178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1324,13 +1250,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1854,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2863,7 +2782,7 @@
       <c r="G113" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2BQWyI+GIPjSwsU51Ogr+zLsNy5hAFSwqNsPq1vw6A5/a/XFm/VZ4Xc41hWVW32h4ZkenK5X6rLMsaQfU8pNtQ==" saltValue="Sq/9h6z2nEPgl7nKKj84LA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="NPK9hUuV8hPU/eNsmabigPrL/wpv3PfbuZQihGQWtrfvsITaBCMHB2GZqJL7zDoKNYNCPbQ2wIlwHb0k8QDnWQ==" saltValue="j1wRNcIfVbe53b2xAKLcow==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="6">
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
@@ -2908,8 +2827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3205,7 +3124,7 @@
       <c r="H19" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="lVUwAhUpZTUAX50Ot5Prt8PYULKNg3NtpKdPBaOeagqhKnol17l4WIl/dJJv2G76kkSWu86USO9WG46WRjKGkQ==" saltValue="CessEHmGHbjq3udPHj78Bw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="o3tXcBN7AKE22SBzetk4apRoLO1qSd2BvQijaOfYNMV92pFbXazGe1Y4OJwaGTEasHHoaahYfdH4p08SYj5Wvw==" saltValue="aeCtQWnikFTwcP0PKFkGkA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="7">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="H13:H17"/>

</xml_diff>